<commit_message>
Benchmark 'openai' for GPT-4o
</commit_message>
<xml_diff>
--- a/benchmark_logs/GPT-4o/3rd-benchmark-session/custom_no_tool-benchmark.xlsx
+++ b/benchmark_logs/GPT-4o/3rd-benchmark-session/custom_no_tool-benchmark.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,35 +481,45 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>Web Search Mode</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Web Query</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Attack Type</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Number of Proposed Services</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Input Tokens</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Output Tokens</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Web Search Costs</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Test Iterations</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Number of Containers</t>
         </is>
@@ -550,25 +560,35 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>CVE-2012-1823</t>
         </is>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
         <v>2</v>
       </c>
-      <c r="M2" t="n">
+      <c r="O2" t="n">
         <v>6751</v>
       </c>
-      <c r="N2" t="n">
+      <c r="P2" t="n">
         <v>839</v>
       </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
         <v>0.02527</v>
       </c>
-      <c r="P2" t="n">
+      <c r="R2" t="n">
         <v>10</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="S2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -607,25 +627,35 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>CVE-2016-5734</t>
         </is>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
         <v>3</v>
       </c>
-      <c r="M3" t="n">
+      <c r="O3" t="n">
         <v>6379</v>
       </c>
-      <c r="N3" t="n">
+      <c r="P3" t="n">
         <v>892</v>
       </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
         <v>0.02487</v>
       </c>
-      <c r="P3" t="n">
+      <c r="R3" t="n">
         <v>3</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="S3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -664,25 +694,35 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
           <t>CVE-2018-12613</t>
         </is>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Local File Inclusion (LFI) leading to Remote Code Execution (RCE)</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
         <v>3</v>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>7003</v>
       </c>
-      <c r="N4" t="n">
+      <c r="P4" t="n">
         <v>938</v>
       </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
         <v>0.02689</v>
       </c>
-      <c r="P4" t="n">
+      <c r="R4" t="n">
         <v>3</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="S4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -721,25 +761,35 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
           <t>CVE-2020-7247</t>
         </is>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
         <v>2</v>
       </c>
-      <c r="M5" t="n">
+      <c r="O5" t="n">
         <v>3657</v>
       </c>
-      <c r="N5" t="n">
+      <c r="P5" t="n">
         <v>690</v>
       </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
         <v>0.01604</v>
       </c>
-      <c r="P5" t="n">
+      <c r="R5" t="n">
         <v>10</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="S5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -778,25 +828,35 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
           <t>CVE-2020-11651</t>
         </is>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>remote code execution</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
         <v>4</v>
       </c>
-      <c r="M6" t="n">
+      <c r="O6" t="n">
         <v>5084</v>
       </c>
-      <c r="N6" t="n">
+      <c r="P6" t="n">
         <v>724</v>
       </c>
-      <c r="O6" t="n">
+      <c r="Q6" t="n">
         <v>0.01995</v>
       </c>
-      <c r="P6" t="n">
+      <c r="R6" t="n">
         <v>6</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="S6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -835,25 +895,35 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
           <t>CVE-2020-11652</t>
         </is>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Unauthorized access to sensitive files</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
         <v>3</v>
       </c>
-      <c r="M7" t="n">
+      <c r="O7" t="n">
         <v>4811</v>
       </c>
-      <c r="N7" t="n">
+      <c r="P7" t="n">
         <v>728</v>
       </c>
-      <c r="O7" t="n">
+      <c r="Q7" t="n">
         <v>0.01931</v>
       </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="n">
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -892,25 +962,35 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
           <t>CVE-2021-3129</t>
         </is>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
         <v>6</v>
       </c>
-      <c r="M8" t="n">
+      <c r="O8" t="n">
         <v>6451</v>
       </c>
-      <c r="N8" t="n">
+      <c r="P8" t="n">
         <v>763</v>
       </c>
-      <c r="O8" t="n">
+      <c r="Q8" t="n">
         <v>0.02376</v>
       </c>
-      <c r="P8" t="n">
+      <c r="R8" t="n">
         <v>6</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="S8" t="n">
         <v>3</v>
       </c>
     </row>
@@ -949,25 +1029,35 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
           <t>CVE-2021-28164</t>
         </is>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Information Disclosure</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
         <v>2</v>
       </c>
-      <c r="M9" t="n">
+      <c r="O9" t="n">
         <v>43605</v>
       </c>
-      <c r="N9" t="n">
+      <c r="P9" t="n">
         <v>911</v>
       </c>
-      <c r="O9" t="n">
+      <c r="Q9" t="n">
         <v>0.11812</v>
       </c>
-      <c r="P9" t="n">
+      <c r="R9" t="n">
         <v>3</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="S9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1006,25 +1096,35 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
           <t>CVE-2021-34429</t>
         </is>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Path Traversal</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
         <v>2</v>
       </c>
-      <c r="M10" t="n">
+      <c r="O10" t="n">
         <v>55449</v>
       </c>
-      <c r="N10" t="n">
+      <c r="P10" t="n">
         <v>902</v>
       </c>
-      <c r="O10" t="n">
+      <c r="Q10" t="n">
         <v>0.14764</v>
       </c>
-      <c r="P10" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q10" t="n">
+      <c r="R10" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1063,25 +1163,35 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
           <t>CVE-2021-41773</t>
         </is>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Path Traversal and Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
         <v>2</v>
       </c>
-      <c r="M11" t="n">
+      <c r="O11" t="n">
         <v>34665</v>
       </c>
-      <c r="N11" t="n">
+      <c r="P11" t="n">
         <v>809</v>
       </c>
-      <c r="O11" t="n">
+      <c r="Q11" t="n">
         <v>0.09475</v>
       </c>
-      <c r="P11" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="n">
+      <c r="R11" t="n">
+        <v>1</v>
+      </c>
+      <c r="S11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1120,25 +1230,35 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
           <t>CVE-2021-42013</t>
         </is>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Path Traversal and Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
         <v>2</v>
       </c>
-      <c r="M12" t="n">
+      <c r="O12" t="n">
         <v>33993</v>
       </c>
-      <c r="N12" t="n">
+      <c r="P12" t="n">
         <v>899</v>
       </c>
-      <c r="O12" t="n">
+      <c r="Q12" t="n">
         <v>0.09397</v>
       </c>
-      <c r="P12" t="n">
+      <c r="R12" t="n">
         <v>9</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="S12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1177,25 +1297,35 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
           <t>CVE-2021-43798</t>
         </is>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Path Traversal</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
         <v>3</v>
       </c>
-      <c r="M13" t="n">
+      <c r="O13" t="n">
         <v>12184</v>
       </c>
-      <c r="N13" t="n">
+      <c r="P13" t="n">
         <v>1097</v>
       </c>
-      <c r="O13" t="n">
+      <c r="Q13" t="n">
         <v>0.04143</v>
       </c>
-      <c r="P13" t="n">
+      <c r="R13" t="n">
         <v>6</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="S13" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1234,25 +1364,35 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
           <t>CVE-2021-44228</t>
         </is>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
         <v>3</v>
       </c>
-      <c r="M14" t="n">
+      <c r="O14" t="n">
         <v>15469</v>
       </c>
-      <c r="N14" t="n">
+      <c r="P14" t="n">
         <v>931</v>
       </c>
-      <c r="O14" t="n">
+      <c r="Q14" t="n">
         <v>0.04798</v>
       </c>
-      <c r="P14" t="n">
+      <c r="R14" t="n">
         <v>3</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="S14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1291,25 +1431,35 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
           <t>CVE-2022-22947</t>
         </is>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Code Injection, Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
         <v>4</v>
       </c>
-      <c r="M15" t="n">
+      <c r="O15" t="n">
         <v>4781</v>
       </c>
-      <c r="N15" t="n">
+      <c r="P15" t="n">
         <v>769</v>
       </c>
-      <c r="O15" t="n">
+      <c r="Q15" t="n">
         <v>0.01964</v>
       </c>
-      <c r="P15" t="n">
+      <c r="R15" t="n">
         <v>8</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="S15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1348,25 +1498,35 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
           <t>CVE-2022-22963</t>
         </is>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
         <v>4</v>
       </c>
-      <c r="M16" t="n">
+      <c r="O16" t="n">
         <v>7068</v>
       </c>
-      <c r="N16" t="n">
+      <c r="P16" t="n">
         <v>724</v>
       </c>
-      <c r="O16" t="n">
+      <c r="Q16" t="n">
         <v>0.02491</v>
       </c>
-      <c r="P16" t="n">
+      <c r="R16" t="n">
         <v>4</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="S16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1405,25 +1565,35 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
           <t>CVE-2022-24706</t>
         </is>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
         <v>3</v>
       </c>
-      <c r="M17" t="n">
+      <c r="O17" t="n">
         <v>8573</v>
       </c>
-      <c r="N17" t="n">
+      <c r="P17" t="n">
         <v>759</v>
       </c>
-      <c r="O17" t="n">
+      <c r="Q17" t="n">
         <v>0.02902</v>
       </c>
-      <c r="P17" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q17" t="n">
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1462,25 +1632,35 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
           <t>CVE-2022-46169</t>
         </is>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
         <v>3</v>
       </c>
-      <c r="M18" t="n">
+      <c r="O18" t="n">
         <v>6944</v>
       </c>
-      <c r="N18" t="n">
+      <c r="P18" t="n">
         <v>1013</v>
       </c>
-      <c r="O18" t="n">
+      <c r="Q18" t="n">
         <v>0.02749</v>
       </c>
-      <c r="P18" t="n">
+      <c r="R18" t="n">
         <v>6</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="S18" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1519,25 +1699,35 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
           <t>CVE-2023-23752</t>
         </is>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Information Disclosure</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
         <v>4</v>
       </c>
-      <c r="M19" t="n">
+      <c r="O19" t="n">
         <v>8009</v>
       </c>
-      <c r="N19" t="n">
+      <c r="P19" t="n">
         <v>754</v>
       </c>
-      <c r="O19" t="n">
+      <c r="Q19" t="n">
         <v>0.02756</v>
       </c>
-      <c r="P19" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" t="n">
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1576,25 +1766,35 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
           <t>CVE-2023-42793</t>
         </is>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>unauthenticated remote code execution</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
         <v>3</v>
       </c>
-      <c r="M20" t="n">
+      <c r="O20" t="n">
         <v>19136</v>
       </c>
-      <c r="N20" t="n">
+      <c r="P20" t="n">
         <v>828</v>
       </c>
-      <c r="O20" t="n">
+      <c r="Q20" t="n">
         <v>0.05612</v>
       </c>
-      <c r="P20" t="n">
+      <c r="R20" t="n">
         <v>5</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="S20" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1633,25 +1833,35 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
+          <t>custom_no_tool</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
           <t>CVE-2024-23897</t>
         </is>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Remote Code Execution</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
         <v>4</v>
       </c>
-      <c r="M21" t="n">
+      <c r="O21" t="n">
         <v>10957</v>
       </c>
-      <c r="N21" t="n">
+      <c r="P21" t="n">
         <v>843</v>
       </c>
-      <c r="O21" t="n">
+      <c r="Q21" t="n">
         <v>0.03582</v>
       </c>
-      <c r="P21" t="n">
+      <c r="R21" t="n">
         <v>6</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="S21" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>